<commit_message>
wip: amended mapping and work on profile
</commit_message>
<xml_diff>
--- a/Mappings/SkinDisorder - STU3.xlsx
+++ b/Mappings/SkinDisorder - STU3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" activeTab="4"/>
+    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="188">
   <si>
     <t>Subject</t>
   </si>
@@ -576,9 +576,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>.valueCodeableConcept</t>
-  </si>
-  <si>
     <t>equal</t>
   </si>
   <si>
@@ -601,12 +598,21 @@
   <si>
     <t>.onsetDateTime</t>
   </si>
+  <si>
+    <t>.code</t>
+  </si>
+  <si>
+    <t>Messes with the cardinality. In zib this item is not 1..1, but in the Condition Resource it is. Still best fit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95320005 (SNOMED) will be in .category</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -653,6 +659,19 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -745,7 +764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -795,9 +814,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -806,6 +822,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1732,7 +1760,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1773,7 +1801,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1814,7 +1842,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11282,7 +11310,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11419,10 +11449,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -11779,7 +11809,7 @@
       <c r="D12" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="22" t="s">
         <v>174</v>
       </c>
     </row>
@@ -16710,8 +16740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16802,15 +16832,17 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
+      <c r="R3" s="25" t="s">
+        <v>187</v>
+      </c>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B4" s="11"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="27" t="s">
         <v>75</v>
       </c>
       <c r="D4" s="12"/>
@@ -16835,19 +16867,21 @@
       <c r="M4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="21" t="s">
         <v>82</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="P4" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q4" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="Q4" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="R4" s="3"/>
+      <c r="R4" s="21" t="s">
+        <v>186</v>
+      </c>
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
@@ -16880,10 +16914,10 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q5" s="22" t="s">
-        <v>179</v>
+        <v>184</v>
+      </c>
+      <c r="Q5" s="21" t="s">
+        <v>178</v>
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
@@ -16919,10 +16953,10 @@
       <c r="O6" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="P6" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="R6" s="22"/>
+      <c r="P6" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="R6" s="21"/>
       <c r="S6" s="2"/>
     </row>
     <row r="7" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
@@ -16958,11 +16992,11 @@
       <c r="O7" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="P7" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q7" s="22" t="s">
+      <c r="P7" s="21" t="s">
         <v>179</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>178</v>
       </c>
       <c r="R7" s="3"/>
       <c r="S7" s="2"/>
@@ -17000,11 +17034,11 @@
       <c r="O8" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="P8" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q8" s="22" t="s">
-        <v>179</v>
+      <c r="P8" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>178</v>
       </c>
       <c r="R8" s="3"/>
       <c r="S8" s="2"/>
@@ -17040,11 +17074,11 @@
         <v>113</v>
       </c>
       <c r="O9" s="2"/>
-      <c r="P9" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q9" s="22" t="s">
-        <v>179</v>
+      <c r="P9" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>178</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
@@ -17078,11 +17112,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>114</v>
       </c>
     </row>
@@ -17136,15 +17170,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
@@ -17230,9 +17264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17244,15 +17276,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">

</xml_diff>